<commit_message>
updates to be able to read raw SAP data @mac
</commit_message>
<xml_diff>
--- a/data/Global Theme - Resp. Unit Mapping.xlsx
+++ b/data/Global Theme - Resp. Unit Mapping.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andres/Library/Mobile Documents/com~apple~CloudDocs/SARA-GFDRR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84498F0E-D027-F64B-BA67-1E6EA631AA7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE19D529-B00D-4142-9F38-FF30C91D1BBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1680" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-1220" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Theme - Resp. Unit Mappi" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Global Theme - Resp. Unit Mappi'!$A$1:$C$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Global Theme - Resp. Unit Mappi'!$A$1:$C$139</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="177">
   <si>
     <t>Resp. Unit</t>
   </si>
@@ -556,13 +558,19 @@
   </si>
   <si>
     <t>FCV</t>
+  </si>
+  <si>
+    <t>IAFT4</t>
+  </si>
+  <si>
+    <t>SAFA4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -703,6 +711,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1052,12 +1066,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1413,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C139"/>
+  <dimension ref="A1:C141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2028,11 +2043,11 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>34</v>
+      <c r="A57" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C57" t="s">
         <v>91</v>
@@ -2040,10 +2055,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B58" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C58" t="s">
         <v>91</v>
@@ -2051,7 +2066,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>36</v>
       </c>
       <c r="B59" t="s">
         <v>32</v>
@@ -2062,7 +2077,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>121</v>
       </c>
       <c r="B60" t="s">
         <v>32</v>
@@ -2073,7 +2088,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B61" t="s">
         <v>32</v>
@@ -2084,10 +2099,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C62" t="s">
         <v>91</v>
@@ -2106,29 +2121,29 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>148</v>
+        <v>39</v>
+      </c>
+      <c r="B64" t="s">
+        <v>35</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>40</v>
-      </c>
-      <c r="B65" t="s">
-        <v>35</v>
+        <v>148</v>
       </c>
       <c r="C65" t="s">
-        <v>91</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B66" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C66" t="s">
         <v>91</v>
@@ -2136,10 +2151,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B67" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C67" t="s">
         <v>91</v>
@@ -2147,10 +2162,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C68" t="s">
         <v>91</v>
@@ -2158,10 +2173,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>123</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>122</v>
+        <v>150</v>
+      </c>
+      <c r="B69" t="s">
+        <v>32</v>
       </c>
       <c r="C69" t="s">
         <v>91</v>
@@ -2169,10 +2184,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>43</v>
-      </c>
-      <c r="B70" t="s">
-        <v>35</v>
+        <v>123</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="C70" t="s">
         <v>91</v>
@@ -2180,10 +2195,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B71" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C71" t="s">
         <v>91</v>
@@ -2191,18 +2206,18 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>151</v>
+        <v>44</v>
       </c>
       <c r="B72" t="s">
-        <v>134</v>
+        <v>32</v>
       </c>
       <c r="C72" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="B73" t="s">
         <v>134</v>
@@ -2213,29 +2228,29 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B74" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="C74" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B75" t="s">
-        <v>134</v>
+        <v>56</v>
       </c>
       <c r="C75" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B76" t="s">
         <v>134</v>
@@ -2246,15 +2261,18 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>156</v>
+        <v>155</v>
+      </c>
+      <c r="B77" t="s">
+        <v>134</v>
       </c>
       <c r="C77" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C78" t="s">
         <v>157</v>
@@ -2262,21 +2280,18 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>102</v>
-      </c>
-      <c r="B79" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
       <c r="C79" t="s">
-        <v>89</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="B80" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C80" t="s">
         <v>89</v>
@@ -2284,10 +2299,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
       <c r="B81" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C81" t="s">
         <v>89</v>
@@ -2295,21 +2310,21 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="B82" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C82" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>47</v>
+      <c r="A83" s="5" t="s">
+        <v>176</v>
       </c>
       <c r="B83" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C83" t="s">
         <v>89</v>
@@ -2317,10 +2332,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>49</v>
+        <v>159</v>
       </c>
       <c r="B84" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C84" t="s">
         <v>89</v>
@@ -2328,7 +2343,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B85" t="s">
         <v>48</v>
@@ -2339,7 +2354,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>160</v>
+        <v>49</v>
       </c>
       <c r="B86" t="s">
         <v>48</v>
@@ -2350,10 +2365,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>104</v>
+        <v>50</v>
       </c>
       <c r="B87" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C87" t="s">
         <v>89</v>
@@ -2361,10 +2376,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
       <c r="B88" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C88" t="s">
         <v>89</v>
@@ -2372,7 +2387,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="B89" t="s">
         <v>52</v>
@@ -2383,7 +2398,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B90" t="s">
         <v>52</v>
@@ -2394,10 +2409,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B91" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C91" t="s">
         <v>89</v>
@@ -2405,10 +2420,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B92" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C92" t="s">
         <v>89</v>
@@ -2416,10 +2431,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="B93" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C93" t="s">
         <v>89</v>
@@ -2427,10 +2442,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B94" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C94" t="s">
         <v>89</v>
@@ -2438,10 +2453,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>161</v>
       </c>
       <c r="B95" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C95" t="s">
         <v>89</v>
@@ -2449,10 +2464,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B96" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C96" t="s">
         <v>89</v>
@@ -2460,10 +2475,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="B97" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C97" t="s">
         <v>89</v>
@@ -2471,10 +2486,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B98" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C98" t="s">
         <v>89</v>
@@ -2482,10 +2497,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="B99" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C99" t="s">
         <v>89</v>
@@ -2493,10 +2508,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B100" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C100" t="s">
         <v>89</v>
@@ -2504,10 +2519,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B101" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C101" t="s">
         <v>89</v>
@@ -2515,10 +2530,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B102" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="C102" t="s">
         <v>89</v>
@@ -2526,7 +2541,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>162</v>
+        <v>64</v>
       </c>
       <c r="B103" t="s">
         <v>18</v>
@@ -2537,7 +2552,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
       <c r="B104" t="s">
         <v>18</v>
@@ -2548,10 +2563,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B105" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="C105" t="s">
         <v>89</v>
@@ -2559,10 +2574,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>66</v>
+        <v>127</v>
       </c>
       <c r="B106" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C106" t="s">
         <v>89</v>
@@ -2570,10 +2585,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>67</v>
+        <v>163</v>
       </c>
       <c r="B107" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C107" t="s">
         <v>89</v>
@@ -2581,10 +2596,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B108" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C108" t="s">
         <v>89</v>
@@ -2592,10 +2607,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
       <c r="B109" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C109" t="s">
         <v>89</v>
@@ -2603,10 +2618,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B110" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C110" t="s">
         <v>89</v>
@@ -2614,10 +2629,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="B111" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C111" t="s">
         <v>89</v>
@@ -2625,10 +2640,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B112" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C112" t="s">
         <v>89</v>
@@ -2636,10 +2651,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B113" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C113" t="s">
         <v>89</v>
@@ -2647,10 +2662,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B114" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C114" t="s">
         <v>89</v>
@@ -2658,10 +2673,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B115" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C115" t="s">
         <v>89</v>
@@ -2669,10 +2684,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="B116" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C116" t="s">
         <v>89</v>
@@ -2680,10 +2695,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B117" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C117" t="s">
         <v>89</v>
@@ -2691,10 +2706,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="B118" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C118" t="s">
         <v>89</v>
@@ -2702,10 +2717,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B119" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C119" t="s">
         <v>89</v>
@@ -2713,10 +2728,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B120" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C120" t="s">
         <v>89</v>
@@ -2724,7 +2739,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="B121" t="s">
         <v>56</v>
@@ -2735,10 +2750,10 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="B122" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C122" t="s">
         <v>89</v>
@@ -2746,7 +2761,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>79</v>
+        <v>164</v>
       </c>
       <c r="B123" t="s">
         <v>56</v>
@@ -2757,7 +2772,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>80</v>
+        <v>130</v>
       </c>
       <c r="B124" t="s">
         <v>56</v>
@@ -2768,10 +2783,10 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>165</v>
+        <v>79</v>
       </c>
       <c r="B125" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C125" t="s">
         <v>89</v>
@@ -2779,10 +2794,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B126" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C126" t="s">
         <v>89</v>
@@ -2790,10 +2805,10 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B127" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C127" t="s">
         <v>89</v>
@@ -2801,10 +2816,10 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>167</v>
+        <v>81</v>
       </c>
       <c r="B128" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C128" t="s">
         <v>89</v>
@@ -2812,10 +2827,10 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="B129" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C129" t="s">
         <v>89</v>
@@ -2823,7 +2838,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
       <c r="B130" t="s">
         <v>56</v>
@@ -2834,10 +2849,10 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>168</v>
+        <v>131</v>
       </c>
       <c r="B131" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C131" t="s">
         <v>89</v>
@@ -2845,10 +2860,10 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B132" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C132" t="s">
         <v>89</v>
@@ -2856,10 +2871,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="B133" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C133" t="s">
         <v>89</v>
@@ -2867,10 +2882,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>83</v>
       </c>
       <c r="B134" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C134" t="s">
         <v>89</v>
@@ -2878,10 +2893,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B135" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C135" t="s">
         <v>89</v>
@@ -2889,7 +2904,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>86</v>
+        <v>132</v>
       </c>
       <c r="B136" t="s">
         <v>56</v>
@@ -2900,10 +2915,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
       <c r="B137" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C137" t="s">
         <v>89</v>
@@ -2911,10 +2926,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B138" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C138" t="s">
         <v>89</v>
@@ -2922,20 +2937,42 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
+        <v>133</v>
+      </c>
+      <c r="B139" t="s">
+        <v>59</v>
+      </c>
+      <c r="C139" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>87</v>
+      </c>
+      <c r="B140" t="s">
+        <v>59</v>
+      </c>
+      <c r="C140" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>169</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C141" t="s">
         <v>170</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C137" xr:uid="{A4CCC76F-B8ED-4A90-9611-5493BFADF18C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C139">
-      <sortCondition ref="A1:A137"/>
+  <autoFilter ref="A1:C139" xr:uid="{A4CCC76F-B8ED-4A90-9611-5493BFADF18C}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C141">
+      <sortCondition ref="A1:A139"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:B139">
-    <sortCondition ref="B11:B139"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:B141">
+    <sortCondition ref="B11:B141"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>